<commit_message>
Bulk Update (Unclean) : - RSC Meta - Korean Archetype identifier - Sekappy scraping
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/UnlimitedMeta.xlsx
+++ b/Excel_and_CSV/UnlimitedMeta.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="255">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -67,10 +67,13 @@
     <t>72BIC</t>
   </si>
   <si>
-    <t>Cowboy Cactus</t>
-  </si>
-  <si>
-    <t>72Zis</t>
+    <t>Sukuna, Brave and Small</t>
+  </si>
+  <si>
+    <t>6DCAy</t>
+  </si>
+  <si>
+    <t>gdZF2</t>
   </si>
   <si>
     <t>Loxis-Roach Forest</t>
@@ -103,13 +106,26 @@
     <t>61Q1A</t>
   </si>
   <si>
-    <t>Whirlwind Rhinoceroach Forest</t>
-  </si>
-  <si>
-    <t>Whirlwind Rhinoceroach</t>
-  </si>
-  <si>
-    <t>6lZu2</t>
+    <t>Machina Foreset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damian, Drillarm Brawler
+</t>
+  </si>
+  <si>
+    <t>6x2lS</t>
+  </si>
+  <si>
+    <t>Damian, Drillarm Brawler</t>
+  </si>
+  <si>
+    <t>Ladica Forest</t>
+  </si>
+  <si>
+    <t>Ladica, Verdant Claw</t>
+  </si>
+  <si>
+    <t>7E7SS</t>
   </si>
   <si>
     <t>Lockdown Sword</t>
@@ -118,10 +134,10 @@
     <t>Sword</t>
   </si>
   <si>
-    <t>Test of Strength</t>
-  </si>
-  <si>
-    <t>6CnpI</t>
+    <t>Armor of the Stars</t>
+  </si>
+  <si>
+    <t>6LDcA</t>
   </si>
   <si>
     <t>Steadfast Samurai</t>
@@ -139,10 +155,10 @@
     <t>6xPSQ</t>
   </si>
   <si>
-    <t>Sky Commander Celia</t>
-  </si>
-  <si>
-    <t>6Sw1o</t>
+    <t>Sera, Maiden of the Dawn</t>
+  </si>
+  <si>
+    <t>7Ahjy</t>
   </si>
   <si>
     <t>Spartacus Sword</t>
@@ -187,6 +203,21 @@
     <t>76r8i</t>
   </si>
   <si>
+    <t>MistoBay Loop Sword</t>
+  </si>
+  <si>
+    <t>Mistolina &amp; Bayleon</t>
+  </si>
+  <si>
+    <t>7EVso</t>
+  </si>
+  <si>
+    <t>Dramatic Retreat</t>
+  </si>
+  <si>
+    <t>72_IA</t>
+  </si>
+  <si>
     <t>Dimension Shift Rune</t>
   </si>
   <si>
@@ -262,6 +293,21 @@
     <t>6ixR6</t>
   </si>
   <si>
+    <t>Natura Dragon</t>
+  </si>
+  <si>
+    <t>Djeana, the Stouthearted</t>
+  </si>
+  <si>
+    <t>7FEFY</t>
+  </si>
+  <si>
+    <t>Feral Aether</t>
+  </si>
+  <si>
+    <t>6qVZA</t>
+  </si>
+  <si>
     <t>Aggro Shadow</t>
   </si>
   <si>
@@ -280,6 +326,21 @@
     <t>745Mi</t>
   </si>
   <si>
+    <t>Minthe Shadow</t>
+  </si>
+  <si>
+    <t>Gremory, Death Teller</t>
+  </si>
+  <si>
+    <t>6yaPI</t>
+  </si>
+  <si>
+    <t>Minthe of the Underworld</t>
+  </si>
+  <si>
+    <t>6EojI</t>
+  </si>
+  <si>
     <t>Atomy Shadow</t>
   </si>
   <si>
@@ -289,19 +350,70 @@
     <t>63MIS</t>
   </si>
   <si>
-    <t>Minthe Shadow</t>
-  </si>
-  <si>
-    <t>Gremory, Death Teller</t>
-  </si>
-  <si>
-    <t>6yaPI</t>
-  </si>
-  <si>
-    <t>Minthe of the Underworld</t>
-  </si>
-  <si>
-    <t>6EojI</t>
+    <t>Zeus</t>
+  </si>
+  <si>
+    <t>6Cueo</t>
+  </si>
+  <si>
+    <t>Ceres, Bride of the Night</t>
+  </si>
+  <si>
+    <t>7BqzI</t>
+  </si>
+  <si>
+    <t>Ceres OTK Shadow</t>
+  </si>
+  <si>
+    <t>Last Words Shadow</t>
+  </si>
+  <si>
+    <t>Thoth</t>
+  </si>
+  <si>
+    <t>6qy7S</t>
+  </si>
+  <si>
+    <t>Chris, Beyond the Patch</t>
+  </si>
+  <si>
+    <t>7BoX2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None </t>
+  </si>
+  <si>
+    <t>Philosopher Shadow</t>
+  </si>
+  <si>
+    <t>Philosopher of Death</t>
+  </si>
+  <si>
+    <t>74AFC</t>
+  </si>
+  <si>
+    <t>Fatal Order</t>
+  </si>
+  <si>
+    <t>gXuCg</t>
+  </si>
+  <si>
+    <t>Machina Gremory Shadow</t>
+  </si>
+  <si>
+    <t>Nicola, Enduring Steward</t>
+  </si>
+  <si>
+    <t>7Ff6I</t>
+  </si>
+  <si>
+    <t>Machina Shadow</t>
+  </si>
+  <si>
+    <t>Aenea, Creative Amethyst</t>
+  </si>
+  <si>
+    <t>7Ff6S</t>
   </si>
   <si>
     <t>Gremory Shadow</t>
@@ -397,9 +509,6 @@
     <t>Elana Summit Haven</t>
   </si>
   <si>
-    <t>78lSg</t>
-  </si>
-  <si>
     <t>Selena Summit Haven</t>
   </si>
   <si>
@@ -457,13 +566,28 @@
     <t>719Nc</t>
   </si>
   <si>
+    <t>Holy Sanctuary</t>
+  </si>
+  <si>
+    <t>74xJg</t>
+  </si>
+  <si>
     <t>Sanctuary Haven</t>
   </si>
   <si>
-    <t>Holy Sanctuary</t>
-  </si>
-  <si>
-    <t>74xJg</t>
+    <t>Jatelant Haven</t>
+  </si>
+  <si>
+    <t>Jatelant</t>
+  </si>
+  <si>
+    <t>7CboS</t>
+  </si>
+  <si>
+    <t>Garuda, Wings of Paradise</t>
+  </si>
+  <si>
+    <t>6zLEc</t>
   </si>
   <si>
     <t>Artifact Portal</t>
@@ -541,10 +665,16 @@
     <t>Aggro Dragon</t>
   </si>
   <si>
-    <t>Byron, Fullmetal Dragoon</t>
-  </si>
-  <si>
-    <t>6ixQy</t>
+    <t>Darkprison Dragon</t>
+  </si>
+  <si>
+    <t>6uNs6</t>
+  </si>
+  <si>
+    <t>Wyrmfire Engineer</t>
+  </si>
+  <si>
+    <t>73iyC</t>
   </si>
   <si>
     <t>Ambush Sword</t>
@@ -625,29 +755,35 @@
     <t>Whims of Chaos Rune</t>
   </si>
   <si>
-    <t>Jatelant Haven</t>
-  </si>
-  <si>
-    <t>Jatelant</t>
-  </si>
-  <si>
-    <t>7CboS</t>
-  </si>
-  <si>
-    <t>Garuda, Wings of Paradise</t>
-  </si>
-  <si>
-    <t>6zLEc</t>
-  </si>
-  <si>
     <t>Epitaph Blood</t>
+  </si>
+  <si>
+    <t>Mono Blood</t>
+  </si>
+  <si>
+    <t>Mono, Immortal Garnet</t>
+  </si>
+  <si>
+    <t>7G1Wo</t>
+  </si>
+  <si>
+    <t>Machina Portal</t>
+  </si>
+  <si>
+    <t>Belphomet, Ultimate Creator</t>
+  </si>
+  <si>
+    <t>7GoLy</t>
+  </si>
+  <si>
+    <t>gcvky</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -659,12 +795,16 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -681,7 +821,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border/>
     <border>
       <left style="medium">
@@ -696,6 +836,22 @@
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
       </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
     </border>
     <border>
       <left style="medium">
@@ -714,36 +870,51 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1037,10 +1208,10 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -1052,22 +1223,22 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
@@ -1078,126 +1249,126 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
@@ -1208,22 +1379,22 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
@@ -1237,13 +1408,13 @@
         <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>52</v>
@@ -1260,22 +1431,22 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
@@ -1286,126 +1457,126 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="G15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>14</v>
@@ -1416,22 +1587,22 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>14</v>
@@ -1442,22 +1613,22 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>14</v>
@@ -1468,67 +1639,67 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="E20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="B21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
+      <c r="F21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
+      <c r="G21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="5" t="s">
         <v>101</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1537,369 +1708,387 @@
       <c r="F22" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="H24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E24" s="1" t="s">
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="E25" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="G25" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="H25" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
+      <c r="F26" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="G26" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="H26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="B27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="F27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H30" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="10"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F31" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>131</v>
+      <c r="E31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>14</v>
+        <v>148</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>14</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>14</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>14</v>
@@ -1910,100 +2099,100 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>14</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>14</v>
+        <v>166</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>14</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>14</v>
@@ -2014,48 +2203,48 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>28</v>
+        <v>182</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>29</v>
+        <v>183</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>14</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>14</v>
@@ -2065,49 +2254,49 @@
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H43" s="1" t="s">
+      <c r="A43" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>34</v>
+        <v>193</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>14</v>
@@ -2117,49 +2306,49 @@
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>187</v>
+      <c r="A45" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>192</v>
+      <c r="A46" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
@@ -2169,197 +2358,447 @@
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" ht="15.75" customHeight="1">
+      <c r="A56" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" ht="15.75" customHeight="1">
+      <c r="A57" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" ht="15.75" customHeight="1">
+      <c r="A58" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B58" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
+      <c r="C58" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" ht="15.75" customHeight="1">
+      <c r="A59" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G61" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="G62" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
@@ -3297,6 +3736,13 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Update for Dawn of Calamity
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/UnlimitedMeta.xlsx
+++ b/Excel_and_CSV/UnlimitedMeta.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$B$1:$B$272</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$B$1:$B$271</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="259">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -51,13 +51,16 @@
     <t>6pQTI</t>
   </si>
   <si>
-    <t>Divine Smithing</t>
-  </si>
-  <si>
-    <t>6pOlw</t>
-  </si>
-  <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Fairy Forest</t>
+  </si>
+  <si>
+    <t>Noxious Elf</t>
+  </si>
+  <si>
+    <t>7HxbS</t>
   </si>
   <si>
     <t>Aggro Forest</t>
@@ -271,7 +274,7 @@
     <t>6A6RK</t>
   </si>
   <si>
-    <t>Burn Dirt Rune</t>
+    <t>Dirt Rune</t>
   </si>
   <si>
     <t>Orichalcum Golem</t>
@@ -280,10 +283,10 @@
     <t>6awkc</t>
   </si>
   <si>
-    <t>Mirror of Truth</t>
-  </si>
-  <si>
-    <t>6tzEg</t>
+    <t>Adamantine Golem</t>
+  </si>
+  <si>
+    <t>6_djS</t>
   </si>
   <si>
     <t>Item Shop Rune</t>
@@ -469,10 +472,10 @@
     <t>6qy7S</t>
   </si>
   <si>
-    <t>Chris, Beyond the Patch</t>
-  </si>
-  <si>
-    <t>7BoX2</t>
+    <t>Wicked Rebirth</t>
+  </si>
+  <si>
+    <t>7BpFw</t>
   </si>
   <si>
     <t xml:space="preserve">None </t>
@@ -655,30 +658,24 @@
     <t>6NBqI</t>
   </si>
   <si>
+    <t>Selena Summit Haven</t>
+  </si>
+  <si>
+    <t>Selena, Sugarkiss Assasin</t>
+  </si>
+  <si>
+    <t>74zWI</t>
+  </si>
+  <si>
+    <t>Virtuous Aether</t>
+  </si>
+  <si>
+    <t>6reog</t>
+  </si>
+  <si>
     <t>Natura Summit Haven</t>
   </si>
   <si>
-    <t>Virtuous Aether</t>
-  </si>
-  <si>
-    <t>6reog</t>
-  </si>
-  <si>
-    <t>Selena, Sugarkiss Assasin</t>
-  </si>
-  <si>
-    <t>74zWI</t>
-  </si>
-  <si>
-    <t>Selena Summit Haven</t>
-  </si>
-  <si>
-    <t>Natura Selena Summit Haven</t>
-  </si>
-  <si>
-    <t>Natura Haven</t>
-  </si>
-  <si>
     <t>Skillfane Haven</t>
   </si>
   <si>
@@ -754,10 +751,19 @@
     <t>6cQBg</t>
   </si>
   <si>
+    <t>Genesis Artifact Portal</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>Genesis Artifact</t>
+  </si>
+  <si>
+    <t>7KcUo</t>
+  </si>
+  <si>
     <t>Artifact Portal</t>
-  </si>
-  <si>
-    <t>Portal</t>
   </si>
   <si>
     <t>Acceleratium</t>
@@ -791,7 +797,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -806,6 +812,11 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -870,18 +881,30 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -891,6 +914,12 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -899,7 +928,7 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1122,7 +1151,7 @@
     <col customWidth="1" min="2" max="2" width="12.25"/>
     <col customWidth="1" min="3" max="3" width="22.13"/>
     <col customWidth="1" min="4" max="4" width="14.75"/>
-    <col customWidth="1" min="5" max="5" width="22.75"/>
+    <col customWidth="1" min="5" max="5" width="32.75"/>
     <col customWidth="1" min="6" max="6" width="12.25"/>
     <col customWidth="1" min="7" max="7" width="13.13"/>
     <col customWidth="1" min="8" max="8" width="14.5"/>
@@ -1167,867 +1196,867 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>32</v>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>65</v>
+      <c r="E15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="G20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="B21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="D21" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="E21" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="F21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>97</v>
+      <c r="E22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="E24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="B25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="D25" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="E25" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="F25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="H25" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F25" s="5" t="s">
+      <c r="D26" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>14</v>
+      <c r="F26" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>14</v>
+      <c r="E27" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>14</v>
+      <c r="G28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>14</v>
+      <c r="E29" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
+      <c r="G30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="G31" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="G32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>146</v>
+      <c r="G33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="H34" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -2035,129 +2064,129 @@
         <v>148</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>152</v>
+        <v>131</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>14</v>
+        <v>144</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>158</v>
+      <c r="H36" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F38" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>137</v>
+      <c r="G38" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>156</v>
+      <c r="H39" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -2165,337 +2194,337 @@
         <v>166</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>14</v>
+        <v>137</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="G41" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>179</v>
+      <c r="E42" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>181</v>
+        <v>12</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H43" s="13" t="s">
         <v>182</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H45" s="3" t="s">
+      <c r="E45" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G45" s="6" t="s">
         <v>188</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="G46" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F46" s="4" t="s">
+      <c r="H46" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F47" s="2" t="s">
+      <c r="D48" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="G47" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C48" s="9" t="s">
+      <c r="F48" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="B49" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="E48" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="F48" s="9" t="s">
+      <c r="D49" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
+      <c r="F49" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="G49" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="D50" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="C51" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="D51" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="E51" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="1" t="s">
+      <c r="H51" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F52" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>208</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
@@ -2503,155 +2532,155 @@
         <v>210</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E53" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>212</v>
+      <c r="F53" s="13" t="s">
+        <v>209</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D54" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E54" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="F54" s="9" t="s">
+      <c r="E54" s="13" t="s">
         <v>212</v>
       </c>
+      <c r="F54" s="13" t="s">
+        <v>213</v>
+      </c>
       <c r="G54" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F55" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>215</v>
-      </c>
       <c r="G55" s="1" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>217</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D56" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E56" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H56" s="1" t="s">
+      <c r="G56" s="13" t="s">
         <v>217</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="H57" s="13" t="s">
         <v>218</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F58" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="H58" s="9" t="s">
-        <v>215</v>
+      <c r="G58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -2659,365 +2688,340 @@
         <v>219</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D59" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E59" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="E59" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>14</v>
+      <c r="F59" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>215</v>
+      <c r="B60" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>222</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>206</v>
+        <v>12</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>207</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>215</v>
+      <c r="A61" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>227</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>208</v>
+        <v>12</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>223</v>
+      <c r="A62" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>228</v>
+      <c r="A63" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>233</v>
+      <c r="A64" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>233</v>
+      <c r="A65" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E66" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>14</v>
+      <c r="A66" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>241</v>
+      <c r="A67" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>247</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>241</v>
+        <v>248</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>247</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>14</v>
+        <v>248</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>14</v>
+      <c r="A68" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>247</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>14</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B69" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>14</v>
+      <c r="C69" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="G70" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H70" s="14" t="s">
-        <v>14</v>
+      <c r="A70" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D71" s="2" t="s">
+      <c r="A71" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E71" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D72" s="2" t="s">
+      <c r="B71" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="D71" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="G72" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
+      <c r="F71" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" ht="15.75" customHeight="1"/>
     <row r="73" ht="15.75" customHeight="1"/>
     <row r="74" ht="15.75" customHeight="1"/>
     <row r="75" ht="15.75" customHeight="1"/>
@@ -3945,11 +3949,10 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="$B$1:$B$272">
-    <sortState ref="B1:B272">
-      <sortCondition ref="B1:B272"/>
+  <autoFilter ref="$B$1:$B$271">
+    <sortState ref="B1:B271">
+      <sortCondition ref="B1:B271"/>
     </sortState>
   </autoFilter>
   <printOptions/>

</xml_diff>